<commit_message>
python and excel, including working with pandas
</commit_message>
<xml_diff>
--- a/pandas/combined_ciscodata.xlsx
+++ b/pandas/combined_ciscodata.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,237 +434,216 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>device</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>device</t>
+          <t>serial</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>serial</t>
+          <t>ip</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ip</t>
+          <t>region</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>region</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
           <t>firmware</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ciscoios</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>C8293-928F</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>192.168.70.1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>northeast</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>v14.6</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ciscoiosxr</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A7392-123D</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10.0.0.1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>northeast</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>v1.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ciscoiosxe</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>C8233-593A</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>172.6.2.11</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>southwest</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>v3.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>cisconxos</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>B1122-938A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>172.4.2.11</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>south</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>v1.2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>ciscoios</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>C8293-928F</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>192.168.70.1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>northeast</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>C2832-23dB</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>192.168.102.1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>west</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>v14.6</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+    <row r="7">
+      <c r="A7" t="inlineStr">
         <is>
           <t>ciscoiosxr</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>A7392-123D</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>10.0.0.1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>northeast</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>C9878-323F</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10.3.3.1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>west</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>v1.2</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ciscoiosxe</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>C8233-593A</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>172.6.2.11</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>southwest</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>v3.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>cisconxos</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>B1122-938A</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>172.4.2.11</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>south</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>v1.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ciscoios</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>C2832-23dB</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>192.168.102.1</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>west</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>v14.6</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+    <row r="8">
+      <c r="A8" t="inlineStr">
         <is>
           <t>ciscoiosxr</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>C9878-323F</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>10.3.3.1</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>west</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>v1.2</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ciscoiosxr</t>
+          <t>C7673-664E</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>C7673-664E</t>
+          <t>10.66.7.1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10.66.7.1</t>
+          <t>north</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
-        <is>
-          <t>north</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
         <is>
           <t>v1.2</t>
         </is>

</xml_diff>